<commit_message>
First draft wireframe complete
</commit_message>
<xml_diff>
--- a/write-ups/website-wireframe/writeframe-benchmark.xlsx
+++ b/write-ups/website-wireframe/writeframe-benchmark.xlsx
@@ -11,36 +11,60 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="avg">Sheet1!$C$18</definedName>
+    <definedName name="n">Sheet1!$C$11</definedName>
+    <definedName name="n_c">Sheet1!$C$10</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Uniform Allocation</t>
   </si>
   <si>
-    <t>Allloc proportional to pop density</t>
-  </si>
-  <si>
-    <t>Allloc proportional to poverty</t>
-  </si>
-  <si>
     <t>CANOPY</t>
   </si>
   <si>
-    <t>189 courts</t>
-  </si>
-  <si>
-    <t>204787 youth</t>
+    <t>Counts by weight:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Points: </t>
+  </si>
+  <si>
+    <t>courts</t>
+  </si>
+  <si>
+    <t>youth</t>
+  </si>
+  <si>
+    <t>Average Score</t>
+  </si>
+  <si>
+    <t>Weight is considered to be points per 10,000 youth</t>
+  </si>
+  <si>
+    <t>Alloc proportional to poverty</t>
+  </si>
+  <si>
+    <t>Alloc proportional to pop density</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,14 +90,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -83,6 +113,217 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Expected</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Targeting Score by Allocation Method</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$3:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Uniform Allocation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Alloc proportional to pop density</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Alloc proportional to poverty</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CANOPY</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14.292827862880886</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.490219813019394</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.43924179432133</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.235329719529087</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="70589440"/>
+        <c:axId val="63608448"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="70589440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="63608448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="63608448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Targeting Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70589440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C11"/>
+  <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -383,38 +624,134 @@
     <col min="2" max="2" width="27.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3">
+        <f>1*avg*0.33*n/10000</f>
+        <v>14.292827862880886</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <f>1*avg*0.45*n/10000</f>
+        <v>19.490219813019394</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <f>1.5*avg*0.33*n/10000</f>
+        <v>21.43924179432133</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" t="s">
+      <c r="C6">
+        <f>1.5*avg*0.45*n/10000</f>
+        <v>29.235329719529087</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10">
+        <v>189</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11">
+        <v>204787</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" t="s">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>17927</v>
+      </c>
+      <c r="E14" s="1">
+        <f>D14/SUM($D$14:$D$17)</f>
+        <v>0.3762066649878284</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>13811</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" ref="E15:E17" si="0">D15/SUM($D$14:$D$17)</f>
+        <v>0.28983043733736252</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C10" t="s">
+      <c r="D16">
+        <v>8423</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.17676068160832703</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C11" t="s">
-        <v>5</v>
+      <c r="D17">
+        <v>7491</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.15720221606648199</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <f>SUMPRODUCT(C14:C17,E14:E17)</f>
+        <v>2.1149584487534625</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Finished refactoring code: is now working
</commit_message>
<xml_diff>
--- a/write-ups/website-wireframe/writeframe-benchmark.xlsx
+++ b/write-ups/website-wireframe/writeframe-benchmark.xlsx
@@ -192,16 +192,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>14.292827862880886</c:v>
+                  <c:v>12.705790537396121</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.490219813019394</c:v>
+                  <c:v>17.326078005540168</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.43924179432133</c:v>
+                  <c:v>19.058685806094182</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.235329719529087</c:v>
+                  <c:v>25.989117008310249</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -218,11 +218,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="70589440"/>
-        <c:axId val="63608448"/>
+        <c:axId val="75096576"/>
+        <c:axId val="63606720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70589440"/>
+        <c:axId val="75096576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -231,7 +231,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63608448"/>
+        <c:crossAx val="63606720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -239,7 +239,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63608448"/>
+        <c:axId val="63606720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -269,7 +269,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70589440"/>
+        <c:crossAx val="75096576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -616,7 +616,7 @@
   <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -635,7 +635,7 @@
       </c>
       <c r="C3">
         <f>1*avg*0.33*n/10000</f>
-        <v>14.292827862880886</v>
+        <v>12.705790537396121</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -644,7 +644,7 @@
       </c>
       <c r="C4">
         <f>1*avg*0.45*n/10000</f>
-        <v>19.490219813019394</v>
+        <v>17.326078005540168</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -653,7 +653,7 @@
       </c>
       <c r="C5">
         <f>1.5*avg*0.33*n/10000</f>
-        <v>21.43924179432133</v>
+        <v>19.058685806094182</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -662,7 +662,7 @@
       </c>
       <c r="C6">
         <f>1.5*avg*0.45*n/10000</f>
-        <v>29.235329719529087</v>
+        <v>25.989117008310249</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -680,7 +680,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C11">
-        <v>204787</v>
+        <v>182048</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>

</xml_diff>